<commit_message>
final data files and prelim mapping
</commit_message>
<xml_diff>
--- a/data/Data Sources List.xlsx
+++ b/data/Data Sources List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petef\Google Drive\Data Work\git\NC-school-achievement\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322676B2-6CAF-40E3-BB72-DC06DE6E7BC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7337A2BB-E9BF-45FC-BBA1-E9E9134857C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{61B57B1F-4793-4EEF-80D1-38C1C3DA266F}"/>
   </bookViews>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Data Sources</t>
   </si>
   <si>
-    <t>Poverty and Median Income</t>
-  </si>
-  <si>
     <t>https://www.census.gov/data/datasets/2018/demo/saipe/2018-state-and-county.html</t>
   </si>
   <si>
@@ -54,16 +51,96 @@
   </si>
   <si>
     <t>SHIFT NC (Sexual Health Initiatives For Teens) </t>
+  </si>
+  <si>
+    <t>For small sample size counties= population x .031 was used for denominator in determining rate</t>
+  </si>
+  <si>
+    <t>https://demography.osbm.nc.gov/explore/dataset/county-population-estimates-standard-revised/export/?disjunctive.county&amp;disjunctive.population&amp;sort=-year&amp;refine.year=July+1,+2018</t>
+  </si>
+  <si>
+    <t>NC Office of State Budget and Management</t>
+  </si>
+  <si>
+    <t>County Pop 2018</t>
+  </si>
+  <si>
+    <t>https://datacenter.kidscount.org/</t>
+  </si>
+  <si>
+    <t>Annie E Casey</t>
+  </si>
+  <si>
+    <t>Children in concentrated Pov</t>
+  </si>
+  <si>
+    <t>children living in tracts with 30% or more pov rate</t>
+  </si>
+  <si>
+    <t>Lead: percent of children ages 1-2 with elevated blood lead levels = 5 micrograms per deciliter (2013 and later) in North Carolina</t>
+  </si>
+  <si>
+    <t>Elevated lead levels age1-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casey, from </t>
+  </si>
+  <si>
+    <t> North Carolina Department of Health and Human Services, Children's Environmental Health Section: Childhood Lead Poisoning Prevention Program Surveillance Data</t>
+  </si>
+  <si>
+    <t>rate per 1,000 juveniles ages 6-15 years old of delinquent complaints received by court services offices</t>
+  </si>
+  <si>
+    <t>Casey, from ACS 2013-2017</t>
+  </si>
+  <si>
+    <t>Poverty and Median Income 2018</t>
+  </si>
+  <si>
+    <t>Juvenile Delinquency 2018</t>
+  </si>
+  <si>
+    <t>from Casey-- North Carolina Juvenile Justice Section: Juvenile Crime Prevention Council County Data Book.</t>
+  </si>
+  <si>
+    <t>Management Assistance for Child Welfare, Work First, and Food &amp; Nutrition Services in North Carolina (v3.21), University of North Carolina at Chapel Hill Jordan Institute for Families. </t>
+  </si>
+  <si>
+    <t>Child Abuse- substantiated abuse per 1000, 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No parent in workforce </t>
+  </si>
+  <si>
+    <t>Casey, from ACS 2013-2018</t>
+  </si>
+  <si>
+    <t>Head of HH has no high school degree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,13 +163,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,48 +485,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399ED598-C4AE-4E8A-B62C-3A0AE2E9AC3A}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="1" max="1" width="53.21875" customWidth="1"/>
     <col min="2" max="2" width="54.6640625" customWidth="1"/>
     <col min="3" max="3" width="75.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{DE406F41-F0DB-4798-94C0-53D511463C6A}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{096CC957-DE1F-42A2-AA03-E34B1201FA37}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>